<commit_message>
feat : UI작업 + GUI에셋 추가
</commit_message>
<xml_diff>
--- a/RawData/Story_Data.xlsx
+++ b/RawData/Story_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grays\Desktop\Project\Unity\OIlNamProject\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45A93B8-7494-491F-BB10-6E82CB365981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96AD8DC-22DB-4C3A-A38C-777CE56E6F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35040" yWindow="1050" windowWidth="20010" windowHeight="11385" xr2:uid="{85DEEBB6-DF23-40A8-8A68-4400491A39F8}"/>
+    <workbookView xWindow="35250" yWindow="2310" windowWidth="20010" windowHeight="11385" xr2:uid="{85DEEBB6-DF23-40A8-8A68-4400491A39F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,23 +54,6 @@
     <t>콰지직.</t>
   </si>
   <si>
-    <t>\n\n전 세계에 균열이 발생했다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>차원 간의 균열이 열리며\n튀어나온 온갖 마물들은\n그야말로 자연재해였다.</t>
-  </si>
-  <si>
-    <t>하지만,\n인류는 멸망하지 않았다.\n\n균열에서 새어 나오는 마나를 받아들여 특별한 힘을 지니게 된 사람들 덕분이었다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내가 바로 그 힘을 가진\n\n'헌터'다.</t>
-  </si>
-  <si>
-    <t>나는 협회에 소속된 헌터다.\n그것도....\n헌터에 관련된 계약에 허점이 많은 시절에 계약하여 노예와 다름 없는 계약...</t>
-  </si>
-  <si>
     <t>큰 계약금을 제시하여 계약금에 홀린 헌터들을 협회에 묶어놓은 다음, 거액의 빚을 지게 하는 계약.</t>
   </si>
   <si>
@@ -83,13 +66,35 @@
     <t>하지만 빚을 갚기 위해서라도 계속 일을 해야 한다.</t>
   </si>
   <si>
-    <t>(사이렌 소리)하… 또 균열이 발생했다.\n뭔 놈의 마물이 이렇게 하루가 멀다 하고 매일 나오는지 지겹다 지겨워…</t>
-  </si>
-  <si>
-    <t>(전화벨소리)왜?\n(중얼거리며) 아니...학교에서 필요한 준비물이 있는데..\n귀찮게 연락하지 말고, 카드로 사\n(뚝 끊음)\n</t>
-  </si>
-  <si>
     <t>하…귀찮네…</t>
+  </si>
+  <si>
+    <t>&amp;&amp;전 세계에 균열이 발생했다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가 바로 그 힘을 가진&amp;&amp;'헌터'다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나는 협회에 소속된 헌터다.&amp;그것도...&amp;헌터에 관련된 계약에 허점이 많은 시절에 계약하여 노예와 다름 없는 계약...</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(사이렌 소리)하… 또 균열이 발생했다.&amp;뭔 놈의 마물이 이렇게 하루가 멀다 하고 매일 나오는지 지겹다 지겨워…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(전화벨소리)왜?&amp;(중얼거리며) 아니...학교에서 필요한 준비물이 있는데..&amp;귀찮게 연락하지 말고, 카드로 사&amp;(뚝 끊음&amp;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하지만,&amp;인류는 멸망하지 않았다.&amp;&amp;균열에서 새어 나오는 마나를 받아들여 특별한 힘을 지니게 된 사람들 덕분이었다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차원 간의 균열이 열리며&amp;튀어나온 온갖 마물들은&amp;그야말로 자연재해였다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -459,7 +464,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -499,7 +504,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -510,7 +515,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
@@ -521,7 +526,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -532,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
@@ -543,7 +548,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>5</v>
@@ -554,7 +559,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>5</v>
@@ -565,7 +570,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>5</v>
@@ -576,7 +581,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>5</v>
@@ -587,7 +592,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
@@ -598,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>5</v>
@@ -609,7 +614,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>5</v>
@@ -620,7 +625,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>4</v>

</xml_diff>